<commit_message>
for TOT training session
</commit_message>
<xml_diff>
--- a/server/dictionary/dataCollectionPeriod.xlsx
+++ b/server/dictionary/dataCollectionPeriod.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2024ICBT\frameFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2024ICBT ANDY WestNOrth\server\dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE8D8FD-8D94-4043-8586-514AC6ECC2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE81236B-09D2-4DE9-9D8B-C347B3F287A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,14 +411,14 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <f>E2-D2+1</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
for start of Nov 02 Month
</commit_message>
<xml_diff>
--- a/server/dictionary/dataCollectionPeriod.xlsx
+++ b/server/dictionary/dataCollectionPeriod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2024ICBT\server\dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6A2CEB-C4FC-4A91-8B3C-0CC60F788EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC146B2D-1192-450C-A085-556DE5F4F52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>endDate</t>
-  </si>
-  <si>
-    <t>startDate</t>
-  </si>
-  <si>
     <t>October</t>
   </si>
   <si>
@@ -55,6 +49,15 @@
   </si>
   <si>
     <t>no_of_days</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>startDay</t>
+  </si>
+  <si>
+    <t>endDay</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,19 +388,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -408,7 +411,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>22</v>
@@ -419,6 +422,27 @@
       <c r="F2">
         <f>E2-D2+1</f>
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2024</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <f>D3+6</f>
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on Filtered Reports
</commit_message>
<xml_diff>
--- a/server/dictionary/dataCollectionPeriod.xlsx
+++ b/server/dictionary/dataCollectionPeriod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2024ICBT\server\dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC146B2D-1192-450C-A085-556DE5F4F52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A728366-4C8E-4B52-BE2B-6CA27D122DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,11 +438,12 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <f>D3+6</f>
-        <v>17</v>
+        <f>D3+13</f>
+        <v>24</v>
       </c>
       <c r="F3">
-        <v>7</v>
+        <f>E3-D3+1</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manual download export queue
</commit_message>
<xml_diff>
--- a/server/dictionary/dataCollectionPeriod.xlsx
+++ b/server/dictionary/dataCollectionPeriod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2024ICBT\server\dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A728366-4C8E-4B52-BE2B-6CA27D122DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DE5362-8BDC-49EC-B6C6-8AC208CFB24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Year</t>
   </si>
@@ -58,16 +58,25 @@
   </si>
   <si>
     <t>endDay</t>
+  </si>
+  <si>
+    <t>December</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,7 +455,29 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2024</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <f>E4-D4+1</f>
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>